<commit_message>
Last changes to sprint 1 stuff
</commit_message>
<xml_diff>
--- a/Scrum stuff/Aanwezigheidslijst.xlsx
+++ b/Scrum stuff/Aanwezigheidslijst.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11670" windowHeight="4635" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Aanwezigheidslijst" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>Aanwezigheid Project 4</t>
   </si>
@@ -763,7 +763,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
@@ -1034,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1126,7 +1126,9 @@
       <c r="D5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
@@ -1150,7 +1152,9 @@
       <c r="D6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="10"/>
+      <c r="E6" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
@@ -1200,7 +1204,9 @@
       <c r="D8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="10"/>
+      <c r="E8" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
@@ -1224,7 +1230,9 @@
       <c r="D9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" s="12" t="s">
+        <v>22</v>
+      </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>

</xml_diff>